<commit_message>
update comments and cdi data
</commit_message>
<xml_diff>
--- a/stats/data/data_children_n42.xlsx
+++ b/stats/data/data_children_n42.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbang/Dropbox/Other_Research/2019_socpop/SocPop/stats/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07FB1AC5-0E9A-D144-A783-55B332AAE738}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6BE636-47DE-DB4A-9208-ADE56D85B8F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="3080" windowWidth="24280" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="3080" windowWidth="30220" windowHeight="18820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_children_n43" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="210">
   <si>
     <t>id</t>
   </si>
@@ -650,9 +650,6 @@
   </si>
   <si>
     <t>084</t>
-  </si>
-  <si>
-    <t>missing</t>
   </si>
 </sst>
 </file>
@@ -1500,8 +1497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EK43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BA1" workbookViewId="0">
-      <selection activeCell="BD12" sqref="BD12"/>
+    <sheetView tabSelected="1" topLeftCell="DF1" workbookViewId="0">
+      <selection activeCell="DX28" sqref="DX28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8248,9 +8245,7 @@
       <c r="DU17" t="s">
         <v>151</v>
       </c>
-      <c r="DW17" s="4" t="s">
-        <v>210</v>
-      </c>
+      <c r="DW17" s="4"/>
       <c r="DY17" t="s">
         <v>147</v>
       </c>
@@ -9032,9 +9027,7 @@
       <c r="DU19" t="s">
         <v>151</v>
       </c>
-      <c r="DW19" s="4" t="s">
-        <v>210</v>
-      </c>
+      <c r="DW19" s="4"/>
       <c r="DY19" t="s">
         <v>147</v>
       </c>
@@ -12180,9 +12173,7 @@
       <c r="DT27">
         <v>29</v>
       </c>
-      <c r="DW27" s="4" t="s">
-        <v>210</v>
-      </c>
+      <c r="DW27" s="4"/>
       <c r="DY27" t="s">
         <v>147</v>
       </c>
@@ -14738,9 +14729,7 @@
       <c r="BI34">
         <v>401</v>
       </c>
-      <c r="BN34" s="4" t="s">
-        <v>210</v>
-      </c>
+      <c r="BN34" s="4"/>
       <c r="BP34" t="s">
         <v>147</v>
       </c>
@@ -14900,9 +14889,7 @@
       <c r="DT34">
         <v>32</v>
       </c>
-      <c r="DW34" s="4" t="s">
-        <v>210</v>
-      </c>
+      <c r="DW34" s="4"/>
       <c r="DY34" t="s">
         <v>147</v>
       </c>
@@ -15112,9 +15099,7 @@
       <c r="BI35">
         <v>411</v>
       </c>
-      <c r="BN35" s="4" t="s">
-        <v>210</v>
-      </c>
+      <c r="BN35" s="4"/>
       <c r="BP35" t="s">
         <v>147</v>
       </c>

</xml_diff>